<commit_message>
Pushed the complete version of the multipage dashboard app
</commit_message>
<xml_diff>
--- a/assets/complete_set.xlsx
+++ b/assets/complete_set.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROGRAMMING\Dash-App\dash_application\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROGRAMMING\Dash-App\dash_application\Cloud-Based-Heat-Map-for-Area-Segmentation-Covid_19\apps\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65AC76F-0292-4F39-A878-CDC172D0FCFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA25FE40-C88D-4962-B268-92C795A0D670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8850" yWindow="5325" windowWidth="19230" windowHeight="10215" xr2:uid="{CAFA06E3-D2FF-4BA5-AECC-121BC18B8F6B}"/>
+    <workbookView xWindow="4515" yWindow="2835" windowWidth="19230" windowHeight="10215" xr2:uid="{CAFA06E3-D2FF-4BA5-AECC-121BC18B8F6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>County</t>
   </si>
@@ -310,6 +310,12 @@
   </si>
   <si>
     <t>05/18/2020</t>
+  </si>
+  <si>
+    <t>05/19/2020</t>
+  </si>
+  <si>
+    <t>05/20/2020</t>
   </si>
 </sst>
 </file>
@@ -662,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF40C36-3545-4BE3-8F01-51C1B0BD8DE7}">
-  <dimension ref="A1:BR48"/>
+  <dimension ref="A1:BT48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BM2" workbookViewId="0">
-      <selection activeCell="BR2" sqref="BR2"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="BU53" sqref="BU53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +680,7 @@
     <col min="62" max="64" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -885,8 +891,14 @@
       <c r="BR1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -902,8 +914,14 @@
       <c r="BR2">
         <v>309</v>
       </c>
-    </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS2">
+        <v>309</v>
+      </c>
+      <c r="BT2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -919,8 +937,14 @@
       <c r="BR3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS3">
+        <v>7</v>
+      </c>
+      <c r="BT3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -936,8 +960,14 @@
       <c r="BR4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS4">
+        <v>8</v>
+      </c>
+      <c r="BT4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -953,8 +983,14 @@
       <c r="BR5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS5">
+        <v>0</v>
+      </c>
+      <c r="BT5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -970,8 +1006,14 @@
       <c r="BR6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS6">
+        <v>0</v>
+      </c>
+      <c r="BT6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -987,8 +1029,14 @@
       <c r="BR7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS7">
+        <v>2</v>
+      </c>
+      <c r="BT7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1004,8 +1052,14 @@
       <c r="BR8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS8">
+        <v>2</v>
+      </c>
+      <c r="BT8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1021,8 +1075,14 @@
       <c r="BR9">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS9">
+        <v>15</v>
+      </c>
+      <c r="BT9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1038,8 +1098,14 @@
       <c r="BR10">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS10">
+        <v>14</v>
+      </c>
+      <c r="BT10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1055,8 +1121,14 @@
       <c r="BR11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS11">
+        <v>0</v>
+      </c>
+      <c r="BT11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1072,8 +1144,14 @@
       <c r="BR12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS12">
+        <v>1</v>
+      </c>
+      <c r="BT12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1089,8 +1167,14 @@
       <c r="BR13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS13">
+        <v>1</v>
+      </c>
+      <c r="BT13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1106,8 +1190,14 @@
       <c r="BR14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS14">
+        <v>0</v>
+      </c>
+      <c r="BT14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1123,8 +1213,14 @@
       <c r="BR15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS15">
+        <v>0</v>
+      </c>
+      <c r="BT15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1140,8 +1236,14 @@
       <c r="BR16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS16">
+        <v>5</v>
+      </c>
+      <c r="BT16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1157,8 +1259,14 @@
       <c r="BR17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS17">
+        <v>3</v>
+      </c>
+      <c r="BT17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1174,8 +1282,14 @@
       <c r="BR18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS18">
+        <v>0</v>
+      </c>
+      <c r="BT18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1191,8 +1305,14 @@
       <c r="BR19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS19">
+        <v>2</v>
+      </c>
+      <c r="BT19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1208,8 +1328,14 @@
       <c r="BR20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS20">
+        <v>2</v>
+      </c>
+      <c r="BT20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1225,8 +1351,14 @@
       <c r="BR21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS21">
+        <v>0</v>
+      </c>
+      <c r="BT21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1242,8 +1374,14 @@
       <c r="BR22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS22">
+        <v>2</v>
+      </c>
+      <c r="BT22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1259,8 +1397,14 @@
       <c r="BR23">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS23">
+        <v>13</v>
+      </c>
+      <c r="BT23">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1276,8 +1420,14 @@
       <c r="BR24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS24">
+        <v>0</v>
+      </c>
+      <c r="BT24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1293,8 +1443,14 @@
       <c r="BR25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS25">
+        <v>0</v>
+      </c>
+      <c r="BT25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1310,8 +1466,14 @@
       <c r="BR26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS26">
+        <v>0</v>
+      </c>
+      <c r="BT26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1327,8 +1489,14 @@
       <c r="BR27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS27">
+        <v>0</v>
+      </c>
+      <c r="BT27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1344,8 +1512,14 @@
       <c r="BR28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS28">
+        <v>3</v>
+      </c>
+      <c r="BT28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1361,8 +1535,14 @@
       <c r="BR29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS29">
+        <v>0</v>
+      </c>
+      <c r="BT29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1378,8 +1558,14 @@
       <c r="BR30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS30">
+        <v>0</v>
+      </c>
+      <c r="BT30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1395,8 +1581,14 @@
       <c r="BR31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS31">
+        <v>0</v>
+      </c>
+      <c r="BT31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1412,8 +1604,14 @@
       <c r="BR32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS32">
+        <v>2</v>
+      </c>
+      <c r="BT32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1429,8 +1627,14 @@
       <c r="BR33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS33">
+        <v>3</v>
+      </c>
+      <c r="BT33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1446,8 +1650,14 @@
       <c r="BR34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS34">
+        <v>0</v>
+      </c>
+      <c r="BT34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1463,8 +1673,14 @@
       <c r="BR35">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS35">
+        <v>36</v>
+      </c>
+      <c r="BT35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1480,8 +1696,14 @@
       <c r="BR36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS36">
+        <v>0</v>
+      </c>
+      <c r="BT36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1497,8 +1719,14 @@
       <c r="BR37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS37">
+        <v>1</v>
+      </c>
+      <c r="BT37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1514,8 +1742,14 @@
       <c r="BR38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS38">
+        <v>2</v>
+      </c>
+      <c r="BT38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1531,8 +1765,14 @@
       <c r="BR39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS39">
+        <v>1</v>
+      </c>
+      <c r="BT39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1548,8 +1788,14 @@
       <c r="BR40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS40">
+        <v>2</v>
+      </c>
+      <c r="BT40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1565,8 +1811,14 @@
       <c r="BR41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS41">
+        <v>2</v>
+      </c>
+      <c r="BT41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1582,8 +1834,14 @@
       <c r="BR42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS42">
+        <v>2</v>
+      </c>
+      <c r="BT42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1599,8 +1857,14 @@
       <c r="BR43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS43">
+        <v>0</v>
+      </c>
+      <c r="BT43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1616,8 +1880,14 @@
       <c r="BR44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS44">
+        <v>2</v>
+      </c>
+      <c r="BT44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1633,8 +1903,14 @@
       <c r="BR45">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS45">
+        <v>10</v>
+      </c>
+      <c r="BT45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1650,8 +1926,14 @@
       <c r="BR46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS46">
+        <v>1</v>
+      </c>
+      <c r="BT46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1667,8 +1949,14 @@
       <c r="BR47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS47">
+        <v>1</v>
+      </c>
+      <c r="BT47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1683,6 +1971,12 @@
       </c>
       <c r="BR48">
         <v>422</v>
+      </c>
+      <c r="BS48">
+        <v>422</v>
+      </c>
+      <c r="BT48">
+        <v>448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>